<commit_message>
fix: fix allure bug
</commit_message>
<xml_diff>
--- a/tests/test_case_users.xlsx
+++ b/tests/test_case_users.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12280"/>
+    <workbookView windowWidth="25600" windowHeight="10480"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
     <t>调用登录接口</t>
   </si>
   <si>
-    <t>block</t>
+    <t>blocker</t>
   </si>
   <si>
     <t>TC-users-001</t>
@@ -183,7 +183,7 @@
     <t>删除用户</t>
   </si>
   <si>
-    <t>修改用户</t>
+    <t>查找用户</t>
   </si>
   <si>
     <t>module_name</t>
@@ -1174,7 +1174,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1355,7 +1355,7 @@
       <c r="D4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="5">
@@ -1447,7 +1447,7 @@
       <c r="D6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="5">

</xml_diff>